<commit_message>
clean the code up
</commit_message>
<xml_diff>
--- a/reformat.xlsx
+++ b/reformat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresewang/Desktop/python_excel_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresewang/Desktop/excel_project-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6768620-0712-F74B-83D9-77B831CB4EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87402EE-45F5-0549-8CC4-9CD704D053FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="460" windowWidth="16180" windowHeight="18560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="82">
   <si>
     <t>Actual</t>
   </si>
@@ -338,9 +338,6 @@
   </si>
   <si>
     <t>Average comp</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Cost Type</t>
@@ -1833,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C74:C84"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -3240,8 +3237,8 @@
       <c r="D87" s="32">
         <v>44105</v>
       </c>
-      <c r="E87" s="27" t="s">
-        <v>58</v>
+      <c r="E87" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -3291,8 +3288,8 @@
       <c r="D90" s="32">
         <v>44105</v>
       </c>
-      <c r="E90" s="27" t="s">
-        <v>58</v>
+      <c r="E90" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -3342,8 +3339,8 @@
       <c r="D93" s="32">
         <v>44105</v>
       </c>
-      <c r="E93" s="27" t="s">
-        <v>58</v>
+      <c r="E93" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -3661,16 +3658,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
         <v>49</v>
@@ -3681,16 +3678,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
       </c>
       <c r="E2" s="20">
         <v>43800</v>
@@ -3701,16 +3698,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="20">
         <v>43800</v>
@@ -3721,16 +3718,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
       </c>
       <c r="E4" s="20">
         <v>43831</v>
@@ -3741,16 +3738,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="20">
         <v>43831</v>
@@ -3761,16 +3758,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>64</v>
       </c>
       <c r="E6" s="20">
         <v>43862</v>
@@ -3781,16 +3778,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="20">
         <v>43862</v>
@@ -3801,16 +3798,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
       </c>
       <c r="E8" s="20">
         <v>43891</v>
@@ -3821,16 +3818,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="20">
         <v>43891</v>
@@ -3841,16 +3838,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
       </c>
       <c r="E10" s="20">
         <v>43922</v>
@@ -3861,16 +3858,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="20">
         <v>43922</v>
@@ -3881,16 +3878,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
         <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>64</v>
       </c>
       <c r="E12" s="20">
         <v>43952</v>
@@ -3901,16 +3898,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="20">
         <v>43952</v>
@@ -3921,16 +3918,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
         <v>62</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="20">
         <v>43983</v>
@@ -3941,16 +3938,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="20">
         <v>43983</v>
@@ -3961,16 +3958,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="20">
         <v>44105</v>
@@ -3981,16 +3978,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="20">
         <v>44105</v>
@@ -4025,13 +4022,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
         <v>49</v>
@@ -4048,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="20">
         <v>43770</v>
@@ -4059,13 +4056,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="20">
         <v>43770</v>
@@ -4076,13 +4073,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="20">
         <v>43770</v>
@@ -4093,13 +4090,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="20">
         <v>43770</v>
@@ -4110,13 +4107,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="20">
         <v>43770</v>
@@ -4127,13 +4124,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="20">
         <v>43770</v>
@@ -4144,13 +4141,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="20">
         <v>43770</v>
@@ -4161,13 +4158,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="20">
         <v>43770</v>
@@ -4178,13 +4175,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="20">
         <v>43770</v>
@@ -4195,13 +4192,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="20">
         <v>43770</v>
@@ -4212,13 +4209,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="20">
         <v>43770</v>
@@ -4235,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="20">
         <v>43800</v>
@@ -4254,13 +4251,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="20">
         <v>43800</v>
@@ -4279,13 +4276,13 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="20">
         <v>43800</v>
@@ -4304,13 +4301,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="20">
         <v>43800</v>
@@ -4329,13 +4326,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="20">
         <v>43800</v>
@@ -4354,13 +4351,13 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="20">
         <v>43800</v>
@@ -4379,13 +4376,13 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="20">
         <v>43800</v>
@@ -4400,13 +4397,13 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="20">
         <v>43800</v>
@@ -4421,13 +4418,13 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="20">
         <v>43800</v>
@@ -4442,13 +4439,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="20">
         <v>43800</v>
@@ -4463,13 +4460,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="20">
         <v>43800</v>
@@ -4501,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="20">
         <v>43831</v>
@@ -4510,13 +4507,13 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="20">
         <v>43831</v>
@@ -4527,13 +4524,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="20">
         <v>43831</v>
@@ -4545,13 +4542,13 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="20">
         <v>43831</v>
@@ -4563,13 +4560,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="20">
         <v>43831</v>
@@ -4582,13 +4579,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="20">
         <v>43831</v>
@@ -4600,13 +4597,13 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32" s="20">
         <v>43831</v>
@@ -4618,13 +4615,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="20">
         <v>43831</v>
@@ -4636,13 +4633,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="20">
         <v>43831</v>
@@ -4654,13 +4651,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="20">
         <v>43831</v>
@@ -4671,13 +4668,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="20">
         <v>43831</v>
@@ -4699,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="20">
         <v>43862</v>
@@ -4708,13 +4705,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="20">
         <v>43862</v>
@@ -4725,13 +4722,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="20">
         <v>43862</v>
@@ -4742,13 +4739,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="20">
         <v>43862</v>
@@ -4759,13 +4756,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="20">
         <v>43862</v>
@@ -4776,13 +4773,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D43" s="20">
         <v>43862</v>
@@ -4793,13 +4790,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" s="20">
         <v>43862</v>
@@ -4810,13 +4807,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="20">
         <v>43862</v>
@@ -4827,13 +4824,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D46" s="20">
         <v>43862</v>
@@ -4844,13 +4841,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D47" s="20">
         <v>43862</v>
@@ -4861,13 +4858,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D48" s="20">
         <v>43862</v>
@@ -4889,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D50" s="20">
         <v>43891</v>
@@ -4898,13 +4895,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D51" s="20">
         <v>43891</v>
@@ -4915,13 +4912,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D52" s="20">
         <v>43891</v>
@@ -4932,13 +4929,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="20">
         <v>43891</v>
@@ -4949,13 +4946,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" s="20">
         <v>43891</v>
@@ -4966,13 +4963,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D55" s="20">
         <v>43891</v>
@@ -4983,13 +4980,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D56" s="20">
         <v>43891</v>
@@ -5000,13 +4997,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D57" s="20">
         <v>43891</v>
@@ -5017,13 +5014,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D58" s="20">
         <v>43891</v>
@@ -5034,13 +5031,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" s="20">
         <v>43891</v>
@@ -5051,13 +5048,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D60" s="20">
         <v>43891</v>
@@ -5079,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D62" s="20">
         <v>43922</v>
@@ -5088,13 +5085,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D63" s="20">
         <v>43922</v>
@@ -5105,13 +5102,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D64" s="20">
         <v>43922</v>
@@ -5122,13 +5119,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D65" s="20">
         <v>43922</v>
@@ -5139,13 +5136,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66" s="20">
         <v>43922</v>
@@ -5156,13 +5153,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67" s="20">
         <v>43922</v>
@@ -5173,13 +5170,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" s="20">
         <v>43922</v>
@@ -5190,13 +5187,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D69" s="20">
         <v>43922</v>
@@ -5207,13 +5204,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D70" s="20">
         <v>43922</v>
@@ -5224,13 +5221,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D71" s="20">
         <v>43922</v>
@@ -5241,13 +5238,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D72" s="20">
         <v>43922</v>
@@ -5269,7 +5266,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D74" s="20">
         <v>43952</v>
@@ -5278,13 +5275,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D75" s="20">
         <v>43952</v>
@@ -5295,13 +5292,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D76" s="20">
         <v>43952</v>
@@ -5312,13 +5309,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D77" s="20">
         <v>43952</v>
@@ -5329,13 +5326,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D78" s="20">
         <v>43952</v>
@@ -5346,13 +5343,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D79" s="20">
         <v>43952</v>
@@ -5363,13 +5360,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D80" s="20">
         <v>43952</v>
@@ -5380,13 +5377,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D81" s="20">
         <v>43952</v>
@@ -5397,13 +5394,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D82" s="20">
         <v>43952</v>
@@ -5414,13 +5411,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D83" s="20">
         <v>43952</v>
@@ -5431,13 +5428,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D84" s="20">
         <v>43952</v>
@@ -5452,7 +5449,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D86" s="20">
         <v>43983</v>
@@ -5461,13 +5458,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D87" s="20">
         <v>43983</v>
@@ -5478,13 +5475,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D88" s="20">
         <v>43983</v>
@@ -5495,13 +5492,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D89" s="20">
         <v>43983</v>
@@ -5512,13 +5509,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D90" s="20">
         <v>43983</v>
@@ -5529,13 +5526,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D91" s="20">
         <v>43983</v>
@@ -5546,13 +5543,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D92" s="20">
         <v>43983</v>
@@ -5563,13 +5560,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D93" s="20">
         <v>43983</v>
@@ -5580,13 +5577,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D94" s="20">
         <v>43983</v>
@@ -5597,13 +5594,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D95" s="20">
         <v>43983</v>
@@ -5614,13 +5611,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D96" s="20">
         <v>43983</v>
@@ -5635,7 +5632,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D98" s="20">
         <v>44105</v>
@@ -5644,13 +5641,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D99" s="20">
         <v>44105</v>
@@ -5661,13 +5658,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D100" s="20">
         <v>44105</v>
@@ -5678,13 +5675,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D101" s="20">
         <v>44105</v>
@@ -5695,13 +5692,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D102" s="20">
         <v>44105</v>
@@ -5712,13 +5709,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D103" s="20">
         <v>44105</v>
@@ -5729,13 +5726,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D104" s="20">
         <v>44105</v>
@@ -5746,13 +5743,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D105" s="20">
         <v>44105</v>
@@ -5763,13 +5760,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D106" s="20">
         <v>44105</v>
@@ -5780,13 +5777,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D107" s="20">
         <v>44105</v>
@@ -5797,13 +5794,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D108" s="20">
         <v>44105</v>
@@ -5842,12 +5839,12 @@
         <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5861,7 +5858,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5875,7 +5872,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -5889,7 +5886,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -5903,7 +5900,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -5932,7 +5929,7 @@
     <row r="8" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -5946,7 +5943,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -5960,7 +5957,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -5974,7 +5971,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -5988,7 +5985,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -6017,7 +6014,7 @@
     <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -6031,7 +6028,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -6045,7 +6042,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -6059,7 +6056,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -6073,7 +6070,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -6102,7 +6099,7 @@
     <row r="22" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -6116,7 +6113,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -6130,7 +6127,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -6144,7 +6141,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -6158,7 +6155,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -6186,7 +6183,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -6200,7 +6197,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -6214,7 +6211,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -6228,7 +6225,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -6242,7 +6239,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
@@ -6270,7 +6267,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
@@ -6284,7 +6281,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
         <v>0</v>
@@ -6298,7 +6295,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
         <v>0</v>
@@ -6312,7 +6309,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
         <v>0</v>
@@ -6326,7 +6323,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
@@ -6354,7 +6351,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -6368,7 +6365,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -6382,7 +6379,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -6396,7 +6393,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -6410,7 +6407,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -6438,7 +6435,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -6452,7 +6449,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
@@ -6466,7 +6463,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
@@ -6480,7 +6477,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -6494,7 +6491,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>

</xml_diff>